<commit_message>
Added power series fit and R-squared
</commit_message>
<xml_diff>
--- a/results_1024Byte_Mega.xlsx
+++ b/results_1024Byte_Mega.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="results_1024Byte_Mega" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -761,6 +758,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.500568055399677E-2"/>
+                  <c:y val="2.7123127718756941E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>results_1024Byte_Mega!$J$133:$J$151</c:f>
@@ -925,6 +973,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.901782532247235E-2"/>
+                  <c:y val="-1.6443942038506836E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="0070C0"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>results_1024Byte_Mega!$M$76:$M$94</c:f>
@@ -1089,6 +1188,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.500568055399677E-2"/>
+                  <c:y val="5.2048263155475083E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>results_1024Byte_Mega!$L$95:$L$113</c:f>
@@ -1253,6 +1403,61 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.49981786785279E-2"/>
+                  <c:y val="5.6576588204083823E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>results_1024Byte_Mega!$L$114:$L$132</c:f>
@@ -1395,11 +1600,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520257024"/>
-        <c:axId val="520251536"/>
+        <c:axId val="341946528"/>
+        <c:axId val="341945352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520257024"/>
+        <c:axId val="341946528"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1521,12 +1726,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520251536"/>
+        <c:crossAx val="341945352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="520251536"/>
+        <c:axId val="341945352"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1648,7 +1853,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520257024"/>
+        <c:crossAx val="341946528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1666,10 +1871,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.79043989343792642"/>
-          <c:y val="0.35384170112957636"/>
-          <c:w val="8.9192455594213516E-2"/>
-          <c:h val="0.10398686930085288"/>
+          <c:x val="0.15828185392804894"/>
+          <c:y val="0.10273442612689863"/>
+          <c:w val="0.12520145784477615"/>
+          <c:h val="0.22722970365799533"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1858,6 +2063,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.8938961577171272E-2"/>
+                  <c:y val="4.9322398714001583E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>results_1024Byte_Mega!$J$58:$J$75</c:f>
@@ -2016,6 +2272,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.2711305823614158E-3"/>
+                  <c:y val="-2.5292028807817706E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="0070C0"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="0070C0"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>results_1024Byte_Mega!$M$1:$M$19</c:f>
@@ -2180,6 +2487,57 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.4393937599905275E-2"/>
+                  <c:y val="-2.6880394275975019E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>results_1024Byte_Mega!$L$20:$L$38</c:f>
@@ -2344,6 +2702,61 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.038391253724863E-2"/>
+                  <c:y val="4.9771529423873917E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="bg1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>results_1024Byte_Mega!$L$39:$L$57</c:f>
@@ -2486,11 +2899,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520134448"/>
-        <c:axId val="520141504"/>
+        <c:axId val="341941432"/>
+        <c:axId val="341940256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520134448"/>
+        <c:axId val="341941432"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2612,12 +3025,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520141504"/>
+        <c:crossAx val="341940256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="520141504"/>
+        <c:axId val="341940256"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2739,7 +3152,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520134448"/>
+        <c:crossAx val="341941432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2757,10 +3170,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.77661587038462299"/>
-          <c:y val="0.49623579059537976"/>
-          <c:w val="9.6411185443924768E-2"/>
-          <c:h val="0.12379926557623204"/>
+          <c:x val="0.12097677264026205"/>
+          <c:y val="0.14713928924974343"/>
+          <c:w val="0.12949389221084207"/>
+          <c:h val="0.24067738937477109"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -4230,55 +4643,6 @@
 </c:userShapes>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="results_lowend_200x"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="8">
-          <cell r="N8">
-            <v>2.2989999999999999</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="N9">
-            <v>5.85</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="N10">
-            <v>13.933999999999999</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="N11">
-            <v>31.870999999999999</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="N12">
-            <v>73.679000000000002</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="N13">
-            <v>168.18199999999999</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="N14">
-            <v>366.27800000000002</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>

</xml_diff>